<commit_message>
dsa 2 pointers and binary search
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63A76A4-05CE-46DC-A5A5-E8EF93ACB99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BA2A85-CFBA-4C63-A961-9DB5EE3195AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>We apply binary search on the speed, rather than an index location.</t>
+  </si>
+  <si>
+    <t>78. Subsets</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subsets/solutions/27281/a-general-approach-to-backtracking-questions-in-java-subsets-permutations-combination-sum-palindrome-partitioning/</t>
+  </si>
+  <si>
+    <t>11. Container With Most Water</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
   </si>
 </sst>
 </file>
@@ -78,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,14 +119,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -125,14 +155,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E4" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E4" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
-    <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty"/>
+    <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{3EE9083D-0D63-4750-A722-07E106EC8E7D}" name="Pattern"/>
+    <tableColumn id="6" xr3:uid="{A7F8125B-A46D-45A5-A7F7-7B50CAA3589B}" name="Notes"/>
     <tableColumn id="4" xr3:uid="{DE704AFB-97F3-4301-86F4-4553376A5970}" name="Link"/>
-    <tableColumn id="5" xr3:uid="{ADF26966-BF99-4413-BC99-50E1713332B4}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -401,18 +431,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="165" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -426,27 +457,52 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dsa graphs and 2 pointers
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BA2A85-CFBA-4C63-A961-9DB5EE3195AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F041F1-F262-4BB5-8DB0-70448AF8077D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33255" yWindow="2595" windowWidth="21600" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Question</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Binary Search</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/koko-eating-bananas/description/</t>
-  </si>
-  <si>
     <t>We apply binary search on the speed, rather than an index location.</t>
   </si>
   <si>
@@ -63,20 +60,47 @@
     <t>Backtracking</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/subsets/solutions/27281/a-general-approach-to-backtracking-questions-in-java-subsets-permutations-combination-sum-palindrome-partitioning/</t>
-  </si>
-  <si>
     <t>11. Container With Most Water</t>
   </si>
   <si>
     <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>130. Surrounded Regions</t>
+  </si>
+  <si>
+    <t>Graph DFS</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/surrounded-regions/solutions/691675/c-beginner-friendly-boundary-dfs-inplace/</t>
+  </si>
+  <si>
+    <t>Use "Boundary DFS". Note that DFS is still O(mxn) time from a for loop, as long as we track visited.</t>
+  </si>
+  <si>
+    <t>42. Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Cumulative approach. Only consider l_max and r_max at each step, the smaller of the two is the limiting factor. We track water at each step, subtacting the elevation.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/trapping-rain-water/solutions/409175/java-detailed-explanations-illustrations-divide-and-conquer-dp-two-pointers/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/subsets/solutions/27281/a-general-approach-to-backtracking-questions-in-java-subsets-permutations-combination-sum-palindrome-partitioning/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/koko-eating-bananas/description/ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +116,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +135,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,15 +154,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -155,8 +197,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E4" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E4" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E6" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -431,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,41 +516,81 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{67C889D1-3FCF-46F6-8BA2-E44E44B7A806}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{34AF42B2-F7C3-444F-9437-E4DD902D8E3B}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{33411E88-F8DD-4E5F-B657-74CCC74E6087}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{1BC867A0-C11D-4912-997B-3C024C8BBA1B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa binary search and stacks
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583BAE29-496F-4A12-868F-D415D62A0A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787A6EAF-CFC4-4123-A7E2-C950BA6DABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Question</t>
   </si>
@@ -109,6 +109,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/single-number/solutions/1772139/c-explained-everything-w-why-xor-works-brute-force-to-optimized-step-by-step-dry-run/ </t>
+  </si>
+  <si>
+    <t>153. Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>We consider where the pivot is in left and right portions, and need a basic check for an already sorted portion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/solutions/158940/beat-100-very-simple-python-very-detailed-explanation/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/generate-parentheses/solutions/10391/java-solution-using-stack/ </t>
+  </si>
+  <si>
+    <t>22. Generate Parentheses</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Custom class and stack, track string, # of open and closed parentheses per step. Use DFS loop.</t>
   </si>
 </sst>
 </file>
@@ -219,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E7" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E9" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -495,15 +516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
@@ -620,6 +641,40 @@
         <v>27</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{67C889D1-3FCF-46F6-8BA2-E44E44B7A806}"/>
@@ -627,10 +682,12 @@
     <hyperlink ref="E3" r:id="rId3" xr:uid="{33411E88-F8DD-4E5F-B657-74CCC74E6087}"/>
     <hyperlink ref="E2" r:id="rId4" xr:uid="{1BC867A0-C11D-4912-997B-3C024C8BBA1B}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{1E718499-25E1-441F-847B-8652990868AB}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{820D0F9C-F5FC-4E8B-B4A5-93051FD1326B}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{9BA49F7F-4CAC-4DBD-A253-07CC0A09022B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa backtracking, lists, bits
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787A6EAF-CFC4-4123-A7E2-C950BA6DABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B801C00-8DF6-4566-B83B-8FB11F2564E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Question</t>
   </si>
@@ -130,6 +130,36 @@
   </si>
   <si>
     <t>Custom class and stack, track string, # of open and closed parentheses per step. Use DFS loop.</t>
+  </si>
+  <si>
+    <t>191. Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>Bit Shifting: While n != 0, count += (n&amp;1), unsigned right shift (&gt;&gt;&gt;) by 1. Optimal solution is n = n &amp; (n-1) without shifting.</t>
+  </si>
+  <si>
+    <t>19. Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/number-of-1-bits/solutions/55099/simple-java-solution-bit-shifting/ </t>
+  </si>
+  <si>
+    <t>Fast and Slow pointers, move fast n ahead, slow.next = slow.next.next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/remove-nth-node-from-end-of-list/solutions/1164542/js-python-java-c-easy-two-pointer-solution-w-explanation/ </t>
+  </si>
+  <si>
+    <t>90. Subsets 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/subsets-ii/solutions/388566/subsets-i-ii-java-solution-with-detailed-explanation-and-comments-recursion-iteration/ </t>
+  </si>
+  <si>
+    <t>Power Set, skip iterations with duplicate previous element.</t>
   </si>
 </sst>
 </file>
@@ -240,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E9" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E12" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E12" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -516,17 +546,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="165" bestFit="1" customWidth="1"/>
   </cols>
@@ -673,6 +703,57 @@
       </c>
       <c r="E9" s="3" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -684,10 +765,13 @@
     <hyperlink ref="E7" r:id="rId5" xr:uid="{1E718499-25E1-441F-847B-8652990868AB}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{820D0F9C-F5FC-4E8B-B4A5-93051FD1326B}"/>
     <hyperlink ref="E9" r:id="rId7" xr:uid="{9BA49F7F-4CAC-4DBD-A253-07CC0A09022B}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{04FB09A1-8EB8-479A-B02B-F862155606BF}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{C7C4F192-0AD1-4F87-A820-28F5B48326B8}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{B06B4F0B-6CD1-479B-BC0E-0188888E02DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa bits and lists
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B801C00-8DF6-4566-B83B-8FB11F2564E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDA4BE1-3464-4A82-BB13-1A6DDA6DF19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Question</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>Power Set, skip iterations with duplicate previous element.</t>
+  </si>
+  <si>
+    <t>338. Counting Bits</t>
+  </si>
+  <si>
+    <t>DP with offset power of 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/counting-bits/solutions/79557/how-we-handle-this-question-on-interview-thinking-process-dp-solution/ </t>
+  </si>
+  <si>
+    <t>Two passes: 1. Copy nodes and hashmap, 2. point nodes</t>
+  </si>
+  <si>
+    <t>138. Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/copy-list-with-random-pointer/solutions/43491/a-solution-with-constant-space-complexity-o-1-and-linear-time-complexity-o-n/ </t>
   </si>
 </sst>
 </file>
@@ -270,8 +288,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E12" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E12" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E14" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E14" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -546,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,6 +774,40 @@
         <v>43</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{67C889D1-3FCF-46F6-8BA2-E44E44B7A806}"/>
@@ -768,10 +820,12 @@
     <hyperlink ref="E10" r:id="rId8" xr:uid="{04FB09A1-8EB8-479A-B02B-F862155606BF}"/>
     <hyperlink ref="E11" r:id="rId9" xr:uid="{C7C4F192-0AD1-4F87-A820-28F5B48326B8}"/>
     <hyperlink ref="E12" r:id="rId10" xr:uid="{B06B4F0B-6CD1-479B-BC0E-0188888E02DB}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{C2B1D465-CB43-44CA-9444-60D36E9CB30E}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{54151347-508C-4C1B-8C99-2DF2DA76C0E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa binary search and linked lists
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91A7D35-AD67-47E3-8729-B5C625FB4C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6155655B-F7E0-4D6F-8655-F89536696205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Question</t>
   </si>
@@ -211,6 +211,21 @@
   </si>
   <si>
     <t>Tortoise and the Hare (Floyd's)</t>
+  </si>
+  <si>
+    <t>Visualize graphically the pivot point, look for the most ideal conditions to narrow the search, and reject the rest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/search-in-rotated-sorted-array/solutions/14436/revised-binary-search/ </t>
+  </si>
+  <si>
+    <t>287. Find the Duplicate Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked List Cycle and Floyd's algorithm for cycle start searching (2 phases). Consider the elements as index pointers. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-the-duplicate-number/solutions/1892921/9-approaches-count-hash-in-place-marked-sort-binary-search-bit-mask-fast-slow-pointers/ </t>
   </si>
 </sst>
 </file>
@@ -321,8 +336,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E18" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E18" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E19" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E19" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -597,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,6 +897,15 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -898,6 +922,23 @@
       </c>
       <c r="E18" s="3" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -917,10 +958,12 @@
     <hyperlink ref="E15" r:id="rId13" xr:uid="{838AB99B-DADE-45A3-9ACD-F1530FB8675D}"/>
     <hyperlink ref="E16" r:id="rId14" xr:uid="{679BFF8C-2337-4737-B033-83BFFCF607DA}"/>
     <hyperlink ref="E18" r:id="rId15" xr:uid="{EFEFB475-E12A-4CF8-AAEA-E3575FD99DE1}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{0E6029DC-60FC-49FB-ADE6-581D48832B02}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{779680FF-B359-44BF-AE11-6A3B522CD565}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa linked lists and trees
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77187E5B-8CE0-4CE3-A801-E841381E5784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED5C40-690C-40B2-98DA-E4B3DFB2C421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Question</t>
   </si>
@@ -244,6 +244,27 @@
   </si>
   <si>
     <t>Use dummy node "trick" and Merge 2 Sorted Lists Function. Merge each list in place onto lists[0]. Optimal is the divide and conquer (merge sort).  You need a helper function to recursively call the Merge 2 Lists on each half to reduce it to 1.</t>
+  </si>
+  <si>
+    <t>25. Reverse Nodes in k-Group</t>
+  </si>
+  <si>
+    <t>We need a dummy node and to track kStart and kLast. Consider groups k at a time. If the kth node in the group is null, that is the break condition of the while loop. Use standard reverse code in a function and call iteratively.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/reverse-nodes-in-k-group/solutions/11440/non-recursive-java-solution-and-idea/ </t>
+  </si>
+  <si>
+    <t>1448. Count Good Nodes in Binary Tree</t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/count-good-nodes-in-binary-tree/solutions/635555/java-100-simple-easy-code-using-pre-order-tree-traversal/ </t>
+  </si>
+  <si>
+    <t>Straightforward, call DFS on root. Define DFS preorder function, but track max on the path.</t>
   </si>
 </sst>
 </file>
@@ -354,8 +375,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E21" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E21" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E23" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E23" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -630,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,6 +1012,40 @@
       </c>
       <c r="E21" s="3" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1014,10 +1069,12 @@
     <hyperlink ref="E19" r:id="rId17" xr:uid="{779680FF-B359-44BF-AE11-6A3B522CD565}"/>
     <hyperlink ref="E20" r:id="rId18" xr:uid="{058627D1-004E-4197-99FE-FA1395D34CF4}"/>
     <hyperlink ref="E21" r:id="rId19" xr:uid="{2810D8E6-93E5-47FE-A546-C8FD7F65845A}"/>
+    <hyperlink ref="E22" r:id="rId20" xr:uid="{9181B169-9961-49A6-9CF6-FAE641250968}"/>
+    <hyperlink ref="E23" r:id="rId21" xr:uid="{3A1503FA-8BDB-42B7-B0BB-0E212DA4EE0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa arrays and backtracking
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED5C40-690C-40B2-98DA-E4B3DFB2C421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E25E01-F26D-4465-93CD-04461B7287A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Question</t>
   </si>
@@ -265,6 +265,27 @@
   </si>
   <si>
     <t>Straightforward, call DFS on root. Define DFS preorder function, but track max on the path.</t>
+  </si>
+  <si>
+    <t>40. Combination Sum 2</t>
+  </si>
+  <si>
+    <t>Use distance from target as a loop condition. Sort the array first, and consider prev to handle duplicates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/combination-sum-ii/solutions/16878/combination-sum-i-ii-and-iii-java-solution-see-the-similarities-yourself/ </t>
+  </si>
+  <si>
+    <t>347. Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Bucket sort. Use  counts as indices and numbers as values, and a hashmap to count occurrences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/top-k-frequent-elements/solutions/81602/java-o-n-solution-bucket-sort/ </t>
   </si>
 </sst>
 </file>
@@ -375,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E23" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E23" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E25" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E25" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -651,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,6 +1067,40 @@
       </c>
       <c r="E23" s="3" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1071,10 +1126,12 @@
     <hyperlink ref="E21" r:id="rId19" xr:uid="{2810D8E6-93E5-47FE-A546-C8FD7F65845A}"/>
     <hyperlink ref="E22" r:id="rId20" xr:uid="{9181B169-9961-49A6-9CF6-FAE641250968}"/>
     <hyperlink ref="E23" r:id="rId21" xr:uid="{3A1503FA-8BDB-42B7-B0BB-0E212DA4EE0A}"/>
+    <hyperlink ref="E24" r:id="rId22" xr:uid="{D57C1505-3CD8-4B06-894A-1FFFA412ED79}"/>
+    <hyperlink ref="E25" r:id="rId23" xr:uid="{466C9492-3064-43BB-891D-C77B3A6F181B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa trees and dp
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553592CB-CE1F-42AB-A98A-B142BABFC03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216E5280-E35C-4090-8C5F-9F76F1FE93ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="100">
   <si>
     <t>Question</t>
   </si>
@@ -306,9 +306,6 @@
     <t xml:space="preserve">https://leetcode.com/problems/longest-palindromic-substring/solutions/2921/share-my-java-solution-using-dynamic-programming/ </t>
   </si>
   <si>
-    <t>For palindrome, we take each index as a midpoint and expand outwards.</t>
-  </si>
-  <si>
     <t>238. Product of Array Except Self</t>
   </si>
   <si>
@@ -316,6 +313,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/product-of-array-except-self/solutions/1342916/3-minute-read-mimicking-an-interview/ </t>
+  </si>
+  <si>
+    <t>For palindrome, we take each index as a midpoint and expand outwards. We use a dp[n][n] array to track palindromes starting at i,j, and also a variable for palindrome start and max length. At the end we return s.substring(palindrome_starts_at, palindrome_starts_at + max_len);</t>
+  </si>
+  <si>
+    <t>230. Kth Smallest Element in a BST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/kth-smallest-element-in-a-bst/solutions/63783/two-easiest-in-order-traverse-java/ </t>
+  </si>
+  <si>
+    <t>As BST is already sorted, we can visit all nodes and store in an array to solve, optimally, the BST is already sorted so no array is needed. Use a stack and solve iteratively to immediately return the kth smallest node.</t>
   </si>
 </sst>
 </file>
@@ -426,8 +435,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E28" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E29" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E29" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -702,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1170,7 @@
         <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>92</v>
@@ -1169,7 +1178,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1178,10 +1187,27 @@
         <v>84</v>
       </c>
       <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>96</v>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1212,10 +1238,11 @@
     <hyperlink ref="E26" r:id="rId24" xr:uid="{F1C4EC1A-AFDD-494B-B1FC-A2FA22FEE06E}"/>
     <hyperlink ref="E27" r:id="rId25" xr:uid="{DB844FD8-3D1D-45A1-BEF4-E35708C94256}"/>
     <hyperlink ref="E28" r:id="rId26" xr:uid="{F5910350-B785-44FC-B45C-6EE8606B793A}"/>
+    <hyperlink ref="E29" r:id="rId27" xr:uid="{C9C72F80-F968-4D94-942D-1B3BB757FB18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and arrays
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FADAC7-1650-4E87-9D37-76527F0BB9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F196032-F800-461C-A2F1-A70104349539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>Question</t>
   </si>
@@ -334,6 +334,24 @@
   </si>
   <si>
     <t>Recursive. From Preorder, recursively, the left node is the root, and that same node is at the middle pointer in the Inorder array. We can look for the value to be mid because every value is unique. The optimal solution does not use any arrays.</t>
+  </si>
+  <si>
+    <t>647. Palindromic Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/palindromic-substrings/solutions/105689/java-solution-8-lines-extendpalindrome/comments/1017849 </t>
+  </si>
+  <si>
+    <t>2 passes - Odd and Even. We consider each index as mid and expand outwards, but also consider the next adjacent to capture the even ones. This is the general formula for finding palindromes. The Dynamic Programming solution uses the dp array to track inner windows.</t>
+  </si>
+  <si>
+    <t>36. Valid Sudoku</t>
+  </si>
+  <si>
+    <t>Use a Hash Set for each rule. For the subsquare rule, we use an array [i][j] to get the the subsquare. Divide by 3 on the row and column to get the coordinates and obtain the subsquare it is in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/valid-sudoku/solutions/15472/short-simple-java-using-strings/ </t>
   </si>
 </sst>
 </file>
@@ -444,8 +462,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E30" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E30" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E32" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E32" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -720,9 +738,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -1234,6 +1252,40 @@
       </c>
       <c r="E30" s="3" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1266,10 +1318,12 @@
     <hyperlink ref="E28" r:id="rId26" xr:uid="{F5910350-B785-44FC-B45C-6EE8606B793A}"/>
     <hyperlink ref="E29" r:id="rId27" xr:uid="{C9C72F80-F968-4D94-942D-1B3BB757FB18}"/>
     <hyperlink ref="E30" r:id="rId28" xr:uid="{41016557-6E38-413D-BA8D-B608C90AF9C5}"/>
+    <hyperlink ref="E31" r:id="rId29" xr:uid="{C763F2BE-520C-4400-ABE4-26B2B59200A8}"/>
+    <hyperlink ref="E32" r:id="rId30" xr:uid="{B203F6D4-07B1-4014-A8D5-E8A72BF72AEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and trees
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F196032-F800-461C-A2F1-A70104349539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6864DA1-9921-4280-9F9B-EF543BA7CFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
   <si>
     <t>Question</t>
   </si>
@@ -352,6 +352,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/valid-sudoku/solutions/15472/short-simple-java-using-strings/ </t>
+  </si>
+  <si>
+    <t>91. Decode Ways</t>
+  </si>
+  <si>
+    <t>The decisions come from take as double digits, or single digits. The empy string dp[0] is 1, and dp[1] should consider 0 or 1. The Iteration considers if the single digit is 0 or not, and the double digit if it is in 1-26.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/decode-ways/solutions/30451/evolve-from-recursion-to-dp/ </t>
+  </si>
+  <si>
+    <t>124. Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can only take nodes that contain both of the children as the root of a subtree. This should be compared with the max path from the parent and taking a split. We do not want to consider negative values in the sum, but they are still a part of the path. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/binary-tree-maximum-path-sum/solutions/389609/full-explanation-article-with-pseudo-code-beats-java-100-time-and-100-space-solution/ </t>
   </si>
 </sst>
 </file>
@@ -462,8 +480,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E32" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E32" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E34" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E34" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -738,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,6 +1304,40 @@
       </c>
       <c r="E32" s="3" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1320,10 +1372,13 @@
     <hyperlink ref="E30" r:id="rId28" xr:uid="{41016557-6E38-413D-BA8D-B608C90AF9C5}"/>
     <hyperlink ref="E31" r:id="rId29" xr:uid="{C763F2BE-520C-4400-ABE4-26B2B59200A8}"/>
     <hyperlink ref="E32" r:id="rId30" xr:uid="{B203F6D4-07B1-4014-A8D5-E8A72BF72AEB}"/>
+    <hyperlink ref="E33" r:id="rId31" xr:uid="{06C6FA64-9429-48FE-B883-CDBBD324179D}"/>
+    <hyperlink ref="E34" r:id="rId32" xr:uid="{93DB85FE-EAD4-4CFF-A2C9-D7FD1B8BA8C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
   <tableParts count="1">
-    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa backtracking and dp
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6864DA1-9921-4280-9F9B-EF543BA7CFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5143924F-9488-4457-9E4B-FB9681736229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="121">
   <si>
     <t>Question</t>
   </si>
@@ -370,6 +370,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/binary-tree-maximum-path-sum/solutions/389609/full-explanation-article-with-pseudo-code-beats-java-100-time-and-100-space-solution/ </t>
+  </si>
+  <si>
+    <t>79. Word Search</t>
+  </si>
+  <si>
+    <t>Recursive Backtracking - DFS. Use a Set to not revisit the same position twice in the path. Use 2d grid traversal for pathfinding, call dfs on each 4 directions, but remove the cell after (backtracking).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/word-search/solutions/279279/java-simple-with-explanation/ </t>
+  </si>
+  <si>
+    <t>322. Coin Change</t>
+  </si>
+  <si>
+    <t>dp[0] to dp[amount]. Track the min amount for each value in the range. Arrays.fill() the initial values to amount + 1, and only return at the end if the value does not equal the initial value. Start with the DFS - Backtracking approach and evolve to Top-Down Memoization, then DP Bottom-Up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/coin-change/solutions/778548/c-dp-solution-explained-100-time-100-space/ </t>
   </si>
 </sst>
 </file>
@@ -480,8 +498,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E34" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E34" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E36" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E36" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -756,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,6 +1356,40 @@
       </c>
       <c r="E34" s="3" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1374,11 +1426,13 @@
     <hyperlink ref="E32" r:id="rId30" xr:uid="{B203F6D4-07B1-4014-A8D5-E8A72BF72AEB}"/>
     <hyperlink ref="E33" r:id="rId31" xr:uid="{06C6FA64-9429-48FE-B883-CDBBD324179D}"/>
     <hyperlink ref="E34" r:id="rId32" xr:uid="{93DB85FE-EAD4-4CFF-A2C9-D7FD1B8BA8C0}"/>
+    <hyperlink ref="E35" r:id="rId33" xr:uid="{F4B09142-2699-43D1-A887-89B0BC1287D2}"/>
+    <hyperlink ref="E36" r:id="rId34" xr:uid="{F5DB9C5F-4C3B-42C4-AAE1-6C660182A564}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
   <tableParts count="1">
-    <tablePart r:id="rId34"/>
+    <tablePart r:id="rId36"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa stacks and sliding window
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF293CF-4380-4645-B13C-0D705AF17213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0713B0F6-A202-45B1-85C6-6B04E8AF1BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="137">
   <si>
     <t>Question</t>
   </si>
@@ -415,6 +415,27 @@
   </si>
   <si>
     <t>DFS - Preorder, add Nulls to the String to signal the tree structure. We recursively consider the next 2 neighbors until both are null, that is the base case and a leaf node. Delimit on , during iteration. The optimal and most elegant solution is serialize using DFS and deserialize using BFS.</t>
+  </si>
+  <si>
+    <t>739. Daily Temperatures</t>
+  </si>
+  <si>
+    <t>A Monotonic Stack question. Store "slow" pointer values in stack and search them when "fast" pointer fails to meet a condition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/daily-temperatures/solutions/109832/java-easy-ac-solution-with-stack/ </t>
+  </si>
+  <si>
+    <t>567. Permutation in String</t>
+  </si>
+  <si>
+    <t>Sliding Window</t>
+  </si>
+  <si>
+    <t>Maintain 2 arrays (or hashmaps) for char frequencies, 1 of the target, and 1 of the window. Update the frequencies of the window and check if they match at each iteration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/permutation-in-string/solutions/102588/java-solution-sliding-window/ </t>
   </si>
 </sst>
 </file>
@@ -525,8 +546,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E39" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E39" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E41" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E41" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -801,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,6 +1489,40 @@
       </c>
       <c r="E39" s="3" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1509,11 +1564,13 @@
     <hyperlink ref="E37" r:id="rId35" xr:uid="{6E14CE38-B1F5-4776-B82A-ED6CCFDA120C}"/>
     <hyperlink ref="E38" r:id="rId36" xr:uid="{EB46DF95-97B1-4579-B3D2-D0FF63C9A600}"/>
     <hyperlink ref="E39" r:id="rId37" xr:uid="{6DE3738C-1BEC-431F-A250-55A93A433423}"/>
+    <hyperlink ref="E40" r:id="rId38" xr:uid="{674D149F-85BE-4B5B-AD24-48DC3B95630D}"/>
+    <hyperlink ref="E41" r:id="rId39" xr:uid="{44AAC642-9E4F-4C66-8F74-2C439A2DA74A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
   <tableParts count="1">
-    <tablePart r:id="rId39"/>
+    <tablePart r:id="rId41"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa two pointers practice
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B25ECA3-5DD8-4D22-81EE-D2F68F65CF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26746A13-73A8-4870-BBCD-2A8247AD12EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="170">
   <si>
     <t>Question</t>
   </si>
@@ -537,6 +537,15 @@
   </si>
   <si>
     <t>HashMap 1 pass for the diff to target (complement). Remember containsKey. For each I, get diff = target - nums[i]. Map.containsKey(diff) else map.put(nums[i], i).</t>
+  </si>
+  <si>
+    <t>125. Valid Palindrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/valid-palindrome/solutions/3165353/beats-96-9-well-explained-code-in-java/ </t>
+  </si>
+  <si>
+    <t>Remember s = s.toLowerCase(). Alphanumeric is a-z and 0-9 and can be computed with (c &gt;= 'a' &amp;&amp; c &lt;= 'z') || (c &gt;= '0' &amp;&amp; c &lt;= '9'). Make a helper function. In the while loop to skip over blank characters, use continue; There is also the Character.isLetterOrDigit() if you can remember it. Watch the while loop conditions.</t>
   </si>
 </sst>
 </file>
@@ -647,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E51" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E51" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E52" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E52" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -923,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D56" sqref="D55:D56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,6 +1803,23 @@
       </c>
       <c r="E51" s="3" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1847,11 +1873,12 @@
     <hyperlink ref="E49" r:id="rId47" xr:uid="{1A446F7D-D70C-486F-89AA-30B967E7DA67}"/>
     <hyperlink ref="E50" r:id="rId48" xr:uid="{1C57C5BB-63A9-419F-A629-5E4E6AADCED8}"/>
     <hyperlink ref="E51" r:id="rId49" xr:uid="{EECC962A-CA87-4FB7-B378-2EA535D0642C}"/>
+    <hyperlink ref="E52" r:id="rId50" xr:uid="{D0508FF0-7809-4FB6-98A6-4FE2AF1F555F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
   <tableParts count="1">
-    <tablePart r:id="rId51"/>
+    <tablePart r:id="rId52"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa backtracking and trees practice
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26746A13-73A8-4870-BBCD-2A8247AD12EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3042EC5-9D95-454F-9CBA-0BED79EDC01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="176">
   <si>
     <t>Question</t>
   </si>
@@ -546,6 +546,24 @@
   </si>
   <si>
     <t>Remember s = s.toLowerCase(). Alphanumeric is a-z and 0-9 and can be computed with (c &gt;= 'a' &amp;&amp; c &lt;= 'z') || (c &gt;= '0' &amp;&amp; c &lt;= '9'). Make a helper function. In the while loop to skip over blank characters, use continue; There is also the Character.isLetterOrDigit() if you can remember it. Watch the while loop conditions.</t>
+  </si>
+  <si>
+    <t>51. N-Queens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/n-queens/solutions/3754625/easy-java-solution-recursion-backtracking-detailed-solution-easy-to-understand-notes/ </t>
+  </si>
+  <si>
+    <t>We can iterate each row and implicitly store the row, but we need to check if valid for columns, positive and negative diagonals. At each step in the decision tree, we check the conditions based on the Set. As the rows and columns change by 1 at each step, the negative diagonal (r-c) stays constant. For the positive diagonal (r+c) stays constant. It is best to have the stringbuilding operation in its own function, and checking ifSafe() with cols, positive and negative diagonals in its own function.</t>
+  </si>
+  <si>
+    <t>226. Invert  Binary Tree</t>
+  </si>
+  <si>
+    <t>Remember that when we work with Trees and other Objects in Java, they are typically mutable. We pass them by references (by value), so it allows us to modify the original object. Use standard pre-order traversal DFS, with base case and recursive step, but at the current node, swap the left and right using the swap algorithm. Then return the root.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/invert-binary-tree/solutions/2463600/easy-100-fully-explained-java-c-python-js-c-python3-recursive-iterative/ </t>
   </si>
 </sst>
 </file>
@@ -656,8 +674,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E52" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E52" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E54" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E54" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -932,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,6 +1838,40 @@
       </c>
       <c r="E52" s="3" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>173</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1874,11 +1926,13 @@
     <hyperlink ref="E50" r:id="rId48" xr:uid="{1C57C5BB-63A9-419F-A629-5E4E6AADCED8}"/>
     <hyperlink ref="E51" r:id="rId49" xr:uid="{EECC962A-CA87-4FB7-B378-2EA535D0642C}"/>
     <hyperlink ref="E52" r:id="rId50" xr:uid="{D0508FF0-7809-4FB6-98A6-4FE2AF1F555F}"/>
+    <hyperlink ref="E53" r:id="rId51" xr:uid="{980F1FFF-07B5-4F09-AC2B-9FF6A499749D}"/>
+    <hyperlink ref="E54" r:id="rId52" xr:uid="{66E8B9E3-36FC-49AE-9A88-28B9D30F11C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId51"/>
+  <pageSetup orientation="portrait" r:id="rId53"/>
   <tableParts count="1">
-    <tablePart r:id="rId52"/>
+    <tablePart r:id="rId54"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and greedy
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D860D025-AF29-4A4A-B31B-1634E3563FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624CC066-7676-447F-BC32-17DDAAADEF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="206">
   <si>
     <t>Question</t>
   </si>
@@ -636,6 +636,24 @@
   </si>
   <si>
     <t>HashSet Solution - Create the result as a HashSet. Return a new ArrayList&lt;&gt;(res), to get the set into the ArrayList. Sort the Array, iterate I in a for loop, maintain j as i+1, k as nums.length-1. While j &lt; k, get the sum of all 3, and if it is the target, then add to the result, then j++ and k--. Else, if the sum is greater than 0, decrement k, else if sum is less than 0, increment j. After we sort, we can move the pointer towards 0. There is also the HashMap solution which builds on 2Sum, iterate nums[i] and solve the 2 sum problem for the target = -nums[i]. If the array cannot be sorted, then we need to use the 2Sum solution.</t>
+  </si>
+  <si>
+    <t>300. Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-increasing-subsequence/solutions/74953/java-solution-dp-simple/ </t>
+  </si>
+  <si>
+    <t>Classic DP problem. A subsequence is a sequence that is not necessarily contiguous. Initialize the dp[] with 1 values as default. Maintain a local max var. We perform a nested for loop, outer i from the the right and inner j from the left. If the nums[j] inner value is greater than the outer value nums[i], then consider a new max length for that index dp[i]. Fill dp[i] = Math.max(1+dp[j], dp[i]).</t>
+  </si>
+  <si>
+    <t>763. Partition Labels</t>
+  </si>
+  <si>
+    <t>We care about the last index where each character occurs at, and we can use a HashMap. Do 2 passes: 1. HashMap, 2. Output. We need to update the while loop (it will be a nested while loop) to extend the current partition to cover all the characters that have a last occurrence inside the partition. After i passes j, we find a valid partition and add it to the result list, until i reaches the end of the string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/partition-labels/solutions/1868842/java-c-visually-explaineddddd/ </t>
   </si>
 </sst>
 </file>
@@ -746,8 +764,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E62" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E62" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E64" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E64" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1022,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,6 +2098,40 @@
       </c>
       <c r="E62" s="3" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63" t="s">
+        <v>202</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2144,11 +2196,13 @@
     <hyperlink ref="E60" r:id="rId58" xr:uid="{72028B4D-1B34-4328-A288-627F999CE469}"/>
     <hyperlink ref="E61" r:id="rId59" xr:uid="{8C483AE8-21DD-44F9-A1EB-B4F395F75D24}"/>
     <hyperlink ref="E62" r:id="rId60" xr:uid="{893DD344-309B-4058-A24F-3B97CF5B4683}"/>
+    <hyperlink ref="E63" r:id="rId61" xr:uid="{6A1B70D5-094B-4569-90D0-3A832CA03037}"/>
+    <hyperlink ref="E64" r:id="rId62" xr:uid="{2364B6B1-0564-485F-92E7-7A30FAE8E2B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId61"/>
+  <pageSetup orientation="portrait" r:id="rId63"/>
   <tableParts count="1">
-    <tablePart r:id="rId62"/>
+    <tablePart r:id="rId64"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp, sql, python
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5562B32-4410-428B-91D0-33B058108787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232FB410-F991-4A25-969E-26FB025C84E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="215">
   <si>
     <t>Question</t>
   </si>
@@ -672,6 +672,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/valid-parenthesis-string/solutions/543521/java-count-open-parenthesis-o-n-time-o-1-space-picture-explain/ </t>
+  </si>
+  <si>
+    <t>62. Unique Paths</t>
+  </si>
+  <si>
+    <t>A recursive solution is DFS with a cache[r][c], as res = right + down counts. For the base case, we can choose to define the finish as 1, and define out of bounds as 0. The last row and col should be filled with 1 as there is only 1 possible path. We can set each cell from the base case (end) and fill the cells with the number of paths that can reach the end. You can return the sum of all of them as the result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/unique-paths/solutions/182143/recursive-memoization-and-dynamic-programming-solutions/ </t>
   </si>
 </sst>
 </file>
@@ -782,8 +791,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E66" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E66" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E67" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E67" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1058,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,6 +2193,23 @@
       </c>
       <c r="E66" s="3" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" t="s">
+        <v>213</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2252,11 +2278,12 @@
     <hyperlink ref="E64" r:id="rId62" xr:uid="{2364B6B1-0564-485F-92E7-7A30FAE8E2B7}"/>
     <hyperlink ref="E65" r:id="rId63" xr:uid="{0DAED9B9-BEBC-4B7B-A57E-DFA04BC0F1AC}"/>
     <hyperlink ref="E66" r:id="rId64" xr:uid="{536808C8-F16C-486E-AE8E-53CBB0CBED04}"/>
+    <hyperlink ref="E67" r:id="rId65" xr:uid="{4CDA9A30-0298-4C05-81AE-799976EC2BF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
   <tableParts count="1">
-    <tablePart r:id="rId66"/>
+    <tablePart r:id="rId67"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa heaps and tries
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2542C97-B8A8-4295-82A0-5D1897116D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD3F8F1-1709-4896-AA8E-9D7D248F4E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="238">
   <si>
     <t>Question</t>
   </si>
@@ -738,6 +738,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/design-add-and-search-words-data-structure/solutions/1725327/java-c-python-a-very-well-detailed-explanation/ </t>
+  </si>
+  <si>
+    <t>215. Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>Heaps</t>
+  </si>
+  <si>
+    <t>The naive way is to sort and return len-k. We can solve with n + klogn time with a heap, but the optimal is average O(n) time with Quick Select. We choose a element as a pivot, and iterate the other elements, choosing to place it to the left or the right of the pivot based on the element we chose. Each side of the pivot is the "partition". At the end, we swap the pivot value with the element remaining at the pivot index. We recursively perform this on the partitions until we find the element at length-k.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/kth-largest-element-in-an-array/solutions/60294/solution-explained/ </t>
   </si>
 </sst>
 </file>
@@ -848,8 +860,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E73" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E73" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E74" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E74" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1124,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,6 +2381,23 @@
       </c>
       <c r="E73" s="3" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>234</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
+        <v>235</v>
+      </c>
+      <c r="D74" t="s">
+        <v>236</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2444,11 +2473,12 @@
     <hyperlink ref="E71" r:id="rId69" xr:uid="{48799BC2-96C6-444B-8B8E-02669E0251D5}"/>
     <hyperlink ref="E72" r:id="rId70" xr:uid="{612755BD-60EB-4191-9B5C-04E43F5A4A46}"/>
     <hyperlink ref="E73" r:id="rId71" xr:uid="{EA4113EE-210F-47B8-885A-EF677632D283}"/>
+    <hyperlink ref="E74" r:id="rId72" xr:uid="{CE35531C-EA82-4A1D-8A3E-9E1522E474ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId72"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
   <tableParts count="1">
-    <tablePart r:id="rId73"/>
+    <tablePart r:id="rId74"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa intervals and math
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D599FCE6-BAD6-40C0-9EC5-E485237E068C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CEBE06-E756-455A-BAD9-DEC0DC81D8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="249">
   <si>
     <t>Question</t>
   </si>
@@ -759,6 +759,30 @@
   </si>
   <si>
     <t>Eulerian Path. Keep going forward until you get stuck, then the remaining nodes form cycles which are found on the way back and get merged into that main path. By writing down the path backwards when retreating from recursion, merging the cycles into the main path is easy.</t>
+  </si>
+  <si>
+    <t>56. Merge Intervals</t>
+  </si>
+  <si>
+    <t>Intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/merge-intervals/solutions/1644169/java-simple-steps-explained-simple-sort/ </t>
+  </si>
+  <si>
+    <t>Classic Merge Intervals. First sort the input then iterate through the interval. Draw a number line to help visualize, especially for more difficult interval problems. Remember the comparator: Arrays.sort(intervals, (a,b) -&gt; Integer.compare(a[0],b[0])); and ans.toArray(res); and ArrayList&lt;int[]&gt; ans  = new ArrayList&lt;&gt;(); If you cant remember the conversions, you can manually iterate.</t>
+  </si>
+  <si>
+    <t>48. Rotate Image</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Brute force - Visualize the matrix and note the offsets from the boundaries of the dimensions. There is a matrix flipping algorithm which you can perform 2x, horizontally and vertically.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/rotate-image/solutions/18879/ac-java-in-place-solution-with-explanation-easy-to-understand/ </t>
   </si>
 </sst>
 </file>
@@ -869,8 +893,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E75" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E75" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E77" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E77" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1145,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,6 +2448,40 @@
       </c>
       <c r="E75" s="3" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>241</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>242</v>
+      </c>
+      <c r="D76" t="s">
+        <v>244</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>245</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>246</v>
+      </c>
+      <c r="D77" t="s">
+        <v>247</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2501,11 +2559,13 @@
     <hyperlink ref="E73" r:id="rId71" xr:uid="{EA4113EE-210F-47B8-885A-EF677632D283}"/>
     <hyperlink ref="E74" r:id="rId72" xr:uid="{CE35531C-EA82-4A1D-8A3E-9E1522E474ED}"/>
     <hyperlink ref="E75" r:id="rId73" xr:uid="{97C19B9D-5042-4EBF-97FB-2201714FA78E}"/>
+    <hyperlink ref="E76" r:id="rId74" xr:uid="{5F2917D3-E10D-4525-B52B-A8E36B1DC77A}"/>
+    <hyperlink ref="E77" r:id="rId75" xr:uid="{107E481E-F02D-491C-86D3-6550AAFB78ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId74"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
   <tableParts count="1">
-    <tablePart r:id="rId75"/>
+    <tablePart r:id="rId77"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa graphs, python and sql
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A87D87-0E1F-4F63-AAB8-CDFB2E5F2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833166FA-CBBF-4905-988D-AA7BC25CCC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="255">
   <si>
     <t>Question</t>
   </si>
@@ -792,6 +792,15 @@
   </si>
   <si>
     <t>Use 4 pointers. Shrink the Left and Right, and Top and Bottom boundaries by 1 at each iteration to get to the submatrix. We can use an outer condition of while (left &lt;= right &amp;&amp; top &lt;= bottom). The we do a for loop for left to right, and increment top by 1 after the loop. Then the same from right to left. Then do the bottom row, then left. For traversing left or up, use an if statement to check for dulicates. Handle off by 1 errors.</t>
+  </si>
+  <si>
+    <t>1584. Min Cost to Connect All Points</t>
+  </si>
+  <si>
+    <t>Minimum Spanning Tree - Prim's or Kruskal's algorithm. For Prim's: 1. Create the edges (adjacency list). It will take n-1 edges to connect the nodes without a cycle. For data data structures, need a hash set for visited nodes, and a min heap for the Frontier, with the weight and the node value. We add to the cost when we pick from the frontier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/min-cost-to-connect-all-points/solutions/4045874/94-85-prim-kruskal-with-min-heap/ </t>
   </si>
 </sst>
 </file>
@@ -902,8 +911,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E78" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E78" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E79" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E79" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1178,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,6 +2517,23 @@
       </c>
       <c r="E78" s="3" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>252</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>179</v>
+      </c>
+      <c r="D79" t="s">
+        <v>253</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2588,11 +2614,12 @@
     <hyperlink ref="E76" r:id="rId74" xr:uid="{5F2917D3-E10D-4525-B52B-A8E36B1DC77A}"/>
     <hyperlink ref="E77" r:id="rId75" xr:uid="{107E481E-F02D-491C-86D3-6550AAFB78ED}"/>
     <hyperlink ref="E78" r:id="rId76" xr:uid="{AA8EB26C-4CB8-4C33-8628-7E57E6956E88}"/>
+    <hyperlink ref="E79" r:id="rId77" xr:uid="{BDAE1C8B-CEEC-428F-A322-B85B3D17877E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId77"/>
+  <pageSetup orientation="portrait" r:id="rId78"/>
   <tableParts count="1">
-    <tablePart r:id="rId78"/>
+    <tablePart r:id="rId79"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa math, python, sql
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B78F081-AFFC-46DF-B31E-EF6BFD635ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E173A-954C-4458-8AB2-79BEF4084B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="261">
   <si>
     <t>Question</t>
   </si>
@@ -810,6 +810,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/non-overlapping-intervals/solutions/510140/java-solution-easy-to-understand-not-most-efficient/ </t>
+  </si>
+  <si>
+    <t>73. Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>In the brute force, start with a copy matrix. Read the input, but update the copy, as we do not want it to dynamically update. For an improvement, replace the copy matrix with a row array and column array to mark which rows and columns get set to zero. The optimal, for O(1) space, we put the row array and column array inside the input matrix itself to perform in place, but need 1 extra dedicated variable for the first cell where rows and columns overlap. The reason we can overlap, is because we read the input before we overwrite, so the computation is accurate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/set-matrix-zeroes/solutions/2525398/all-approaches-from-brute-force-to-optimal-with-easy-explanation/ </t>
   </si>
 </sst>
 </file>
@@ -920,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E80" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E80" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E81" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E81" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1196,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,6 +2569,23 @@
       </c>
       <c r="E80" s="3" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>258</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>246</v>
+      </c>
+      <c r="D81" t="s">
+        <v>259</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2642,11 +2668,12 @@
     <hyperlink ref="E78" r:id="rId76" xr:uid="{AA8EB26C-4CB8-4C33-8628-7E57E6956E88}"/>
     <hyperlink ref="E79" r:id="rId77" xr:uid="{BDAE1C8B-CEEC-428F-A322-B85B3D17877E}"/>
     <hyperlink ref="E80" r:id="rId78" xr:uid="{4720461F-13F5-4471-A513-2148328C2006}"/>
+    <hyperlink ref="E81" r:id="rId79" xr:uid="{BAD4C498-C707-47B1-9B1C-D7ED69C9AE86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId79"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
   <tableParts count="1">
-    <tablePart r:id="rId80"/>
+    <tablePart r:id="rId81"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa heaps and math
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6901562-3385-40B7-91E9-160BF9067D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C2E745-CA35-483D-AA69-386607E3CD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="279">
   <si>
     <t>Question</t>
   </si>
@@ -855,6 +855,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/task-scheduler/solutions/104511/java-solution-priorityqueue-and-hashmap/ </t>
+  </si>
+  <si>
+    <t>355. Design Twitter</t>
+  </si>
+  <si>
+    <t>Review. Similar to Merge K Sorted List. 1. Follow/unfollow functions HashMap of UserIds, maps to a HashSet of followeeIds. 2. postTweet is a HashMap of userIds which maps to a list of [count, TweetIds]. 3. Put the time of tweets in a Max Heap for getNewsFeed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/design-twitter/solutions/82825/java-oo-design-with-most-efficient-function-getnewsfeed/ </t>
+  </si>
+  <si>
+    <t>66. Plus One</t>
+  </si>
+  <si>
+    <t>Remember the carry when reaching 10. The crux is to manage 2 potential result arrays, newDigits and the input digits array in place. If there is a carry at the end, we add it to newDigits[0] and then return it, else we just return the input array which we computed in place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/plus-one/solutions/2706861/java-fastest-0ms-runtime-easy-and-elegant-solution/ </t>
   </si>
 </sst>
 </file>
@@ -965,8 +983,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E85" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E85" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E87" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E87" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1241,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,6 +2708,40 @@
       </c>
       <c r="E85" s="3" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>273</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>235</v>
+      </c>
+      <c r="D86" t="s">
+        <v>274</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>276</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" t="s">
+        <v>246</v>
+      </c>
+      <c r="D87" t="s">
+        <v>277</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2777,11 +2829,13 @@
     <hyperlink ref="E83" r:id="rId81" xr:uid="{A1AE87C1-ACB6-474C-9E85-33EC8A7BCDE1}"/>
     <hyperlink ref="E84" r:id="rId82" xr:uid="{A4EA6566-C022-402B-B933-2D8158BE5DBD}"/>
     <hyperlink ref="E85" r:id="rId83" xr:uid="{A4A7A1BD-66B7-4214-A900-B665A9E8AF3F}"/>
+    <hyperlink ref="E86" r:id="rId84" xr:uid="{85935840-A156-42EC-A4B1-59D567D3BF87}"/>
+    <hyperlink ref="E87" r:id="rId85" xr:uid="{611AFF68-67C1-40B1-A2CF-AD717B47F012}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId84"/>
+  <pageSetup orientation="portrait" r:id="rId86"/>
   <tableParts count="1">
-    <tablePart r:id="rId85"/>
+    <tablePart r:id="rId87"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and math
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBDBE63-95C7-4B19-BDD5-2CD545B24EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11259FDD-81D9-44EA-BE4E-B317208D196A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="303">
   <si>
     <t>Question</t>
   </si>
@@ -927,6 +927,24 @@
   </si>
   <si>
     <t>Bellman Ford. It is an extension of BFS. It consists of initializing the initial array to infinity, then iterative relaxation of the edges with a temp copy of the initial array at each layer, to get the minimum cost per step to each node. At the end, we return the cost value at the destination node index in the initial array, which should now be populated with the minimum cost value if a path exists. You can work your way to the solution using DFS, BFS, and Dijkstra's, but this problem is meant to be solved with Bellman Ford, and the others will give a TLE on LC.</t>
+  </si>
+  <si>
+    <t>518. Coin Change 2</t>
+  </si>
+  <si>
+    <t>Unbounded Knapsack Problem. Start with Brute force, recursion with memoization, then bottom-up. The optimal is a Tabular representation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/coin-change-ii/solutions/3892702/100-dynamic-programming-video-optimal-solution/ </t>
+  </si>
+  <si>
+    <t>5877. Detect Squares</t>
+  </si>
+  <si>
+    <t>We store the points in a list.To verify if a square is possible, we check if 2 points form a diagonal, where the height (y difference) is equal to the widgth (x difference). We need to consider duplicates of points as they add possible combinations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/detect-squares/solutions/1472167/java-clean-solution-with-list-and-hashmap/ </t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1055,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E93" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E93" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E95" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E95" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1313,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,6 +2916,40 @@
       </c>
       <c r="E93" s="3" t="s">
         <v>295</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>297</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>90</v>
+      </c>
+      <c r="D94" t="s">
+        <v>298</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>300</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>246</v>
+      </c>
+      <c r="D95" t="s">
+        <v>301</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2992,11 +3044,13 @@
     <hyperlink ref="E91" r:id="rId88" xr:uid="{11AD299E-5BAA-4BA1-91E1-6E08A78E3BDD}"/>
     <hyperlink ref="E92" r:id="rId89" xr:uid="{F2CAF672-895C-4822-A488-E27F82A30877}"/>
     <hyperlink ref="E93" r:id="rId90" xr:uid="{248821E2-00B4-43D6-BECF-232BFD8CAB22}"/>
+    <hyperlink ref="E94" r:id="rId91" xr:uid="{B718EC84-7657-454A-8643-2D5E08D6523B}"/>
+    <hyperlink ref="E95" r:id="rId92" xr:uid="{CE41C08D-7D36-4B78-BFC3-C1B55E112D47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId91"/>
+  <pageSetup orientation="portrait" r:id="rId93"/>
   <tableParts count="1">
-    <tablePart r:id="rId92"/>
+    <tablePart r:id="rId94"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and bits
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11259FDD-81D9-44EA-BE4E-B317208D196A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531E6A4B-F146-42DA-A692-B62CE712CAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="310">
   <si>
     <t>Question</t>
   </si>
@@ -945,6 +945,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/detect-squares/solutions/1472167/java-clean-solution-with-list-and-hashmap/ </t>
+  </si>
+  <si>
+    <t>494. Target Sum</t>
+  </si>
+  <si>
+    <t>At each step (element in nums), there are 2 choices: add the element or subtract it. This forms a binary tree of decisions. We use a hashmap cache to store computations. The base case is when i == nums.length, and if sum equals the target, it is a valid way. The recursive step at each step should add the sum of both recursive calls.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/target-sum/solutions/455024/dp-is-easy-5-steps-to-think-through-dp-questions/ </t>
+  </si>
+  <si>
+    <t>190. Reverse Bits</t>
+  </si>
+  <si>
+    <t>Easay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/reverse-bits/solutions/54738/sharing-my-2ms-java-solution-with-explanation/ </t>
+  </si>
+  <si>
+    <t>Review bit manipulation. To get the current bit, we can AND with 1. To shift the 1 to see the bits to the left, we shift the 1 to the left with &lt;&lt;. To fill the output, we start by shifting 1 to the very left with &lt;&lt; 31, then use OR with (n &amp; 1) to replace the bits with the LSB of n, reversed. The crux is to understand how to work with least significant bits (LSB) as a pointer, left and right shift, Logic OR and Logic AND to get and replace LSBs.</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1076,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E95" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E95" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E97" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E97" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1331,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,6 +2971,40 @@
       </c>
       <c r="E95" s="3" t="s">
         <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>303</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>90</v>
+      </c>
+      <c r="D96" t="s">
+        <v>304</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>306</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C97" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" t="s">
+        <v>309</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3046,11 +3101,13 @@
     <hyperlink ref="E93" r:id="rId90" xr:uid="{248821E2-00B4-43D6-BECF-232BFD8CAB22}"/>
     <hyperlink ref="E94" r:id="rId91" xr:uid="{B718EC84-7657-454A-8643-2D5E08D6523B}"/>
     <hyperlink ref="E95" r:id="rId92" xr:uid="{CE41C08D-7D36-4B78-BFC3-C1B55E112D47}"/>
+    <hyperlink ref="E96" r:id="rId93" xr:uid="{A3950D25-F02D-48B4-B8FD-908BD1F32772}"/>
+    <hyperlink ref="E97" r:id="rId94" xr:uid="{B663C090-EB3B-4193-85E5-0A2283907C12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId93"/>
+  <pageSetup orientation="portrait" r:id="rId95"/>
   <tableParts count="1">
-    <tablePart r:id="rId94"/>
+    <tablePart r:id="rId96"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp finish nc150
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC50ECF-4C4A-4B19-98FD-EAB32B0F4FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4D5091-8845-4D25-9B4A-FE28442A35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="336">
   <si>
     <t>Question</t>
   </si>
@@ -1035,6 +1035,15 @@
   </si>
   <si>
     <t>Review. The Brute Force solution is the decision tree O(N^n). The crux is to consider for the balloons to compute what happens if it is popped last, for the purpose of the dp array. The time complexity of the optimal is O(n^3) and O(n^2) space.</t>
+  </si>
+  <si>
+    <t>10. Regular Expression Matching</t>
+  </si>
+  <si>
+    <t>The crux is to use the indices of the strings to perform the operations. In the cache, we can store valid or invalid up to that point. In the base case, recognize that if index j reaches the end only, then we have exhausted the characters in p, the String  we use to match, therefore the check should return false. There are 3 core logics to code: 1. Matching characters: s(i) and p(j) are matching OR p(j) is '.' 2. p(j) is '*': 2.a. We can choose to not use the '*', or empty set. We skip both its preceding char and the '*'. 2.b. We do take the '*' and its preceding character, by i+1 and j. Moving past j will be handled in subsequent calls. Note that we check j+1 at each step for the occurrence of '*'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/regular-expression-matching/solutions/5847/evolve-from-brute-force-to-dp/ </t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1157,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E105" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E105" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E106" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E106" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1424,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+      <selection activeCell="D111" sqref="D110:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3213,6 +3222,23 @@
       </c>
       <c r="E105" s="3" t="s">
         <v>331</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>333</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" t="s">
+        <v>90</v>
+      </c>
+      <c r="D106" t="s">
+        <v>334</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -3319,11 +3345,12 @@
     <hyperlink ref="E103" r:id="rId100" xr:uid="{F9874DD5-86F8-43F1-913A-F44432B85BDD}"/>
     <hyperlink ref="E104" r:id="rId101" xr:uid="{0E450A26-1D93-4612-9D4A-FD1E5D2CEF6C}"/>
     <hyperlink ref="E105" r:id="rId102" xr:uid="{ED05E0E4-D757-405E-A527-46E3B16D41A6}"/>
+    <hyperlink ref="E106" r:id="rId103" xr:uid="{1CF22A4F-D258-45B2-ABBD-F76220634F81}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId103"/>
+  <pageSetup orientation="portrait" r:id="rId104"/>
   <tableParts count="1">
-    <tablePart r:id="rId104"/>
+    <tablePart r:id="rId105"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa trees and binary search
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4D5091-8845-4D25-9B4A-FE28442A35DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DA89F4-AAB8-4E8B-9E37-D378EC5F126B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="342">
   <si>
     <t>Question</t>
   </si>
@@ -215,9 +215,6 @@
     <t>141. Linked List Cycle</t>
   </si>
   <si>
-    <t>Tortoise and the Hare (Floyd's)</t>
-  </si>
-  <si>
     <t>Visualize graphically the pivot point, look for the most ideal conditions to narrow the search, and reject the rest.</t>
   </si>
   <si>
@@ -1044,6 +1041,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/regular-expression-matching/solutions/5847/evolve-from-brute-force-to-dp/ </t>
+  </si>
+  <si>
+    <t>Tortoise and the Hare (Floyd's). Remember to use fast and fast.next for the null checks, as it is moving first. The loop should contain fast.next.next.</t>
+  </si>
+  <si>
+    <t>104. Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Perform recursive DFS on left and right, and return the maximum + 1 (the node itself). The base case is the null node.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-depth-of-binary-tree/solutions/1769344/java-c-easy-to-go-explanation-solution/ </t>
+  </si>
+  <si>
+    <t>704. Binary Search</t>
+  </si>
+  <si>
+    <t>Classic Binary Search. You should know this in your sleep. Generally, use while (l &lt;= r) for outer loop, and for partitions use l = mid + 1 and r = mid - 1. Note that calculating mid gives TLE if you use (l+(r-l))/2 instead of l+(r-l)/2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/binary-search/solutions/423162/binary-search-101/ </t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1175,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E106" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E106" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E108" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E108" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -1433,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="D111" sqref="D110:D111"/>
+    <sheetView tabSelected="1" topLeftCell="B92" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1533,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -1705,7 +1723,7 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>55</v>
@@ -1722,10 +1740,10 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,7 +1757,7 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>335</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>57</v>
@@ -1747,7 +1765,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -1756,15 +1774,15 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
@@ -1773,15 +1791,15 @@
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>17</v>
@@ -1790,15 +1808,15 @@
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>17</v>
@@ -1807,32 +1825,32 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
@@ -1841,185 +1859,185 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>83</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" t="s">
-        <v>101</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
@@ -2028,32 +2046,32 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
         <v>117</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
@@ -2062,49 +2080,49 @@
         <v>50</v>
       </c>
       <c r="D37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>6</v>
@@ -2113,32 +2131,32 @@
         <v>32</v>
       </c>
       <c r="D40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>133</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>6</v>
@@ -2147,15 +2165,15 @@
         <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>6</v>
@@ -2164,15 +2182,15 @@
         <v>7</v>
       </c>
       <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>17</v>
@@ -2181,15 +2199,15 @@
         <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>17</v>
@@ -2198,49 +2216,49 @@
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
+        <v>148</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>6</v>
@@ -2249,32 +2267,32 @@
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>6</v>
@@ -2283,32 +2301,32 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>23</v>
@@ -2317,15 +2335,15 @@
         <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>17</v>
@@ -2334,66 +2352,66 @@
         <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" t="s">
-        <v>90</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>177</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>179</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>23</v>
@@ -2402,15 +2420,15 @@
         <v>37</v>
       </c>
       <c r="D57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>6</v>
@@ -2419,32 +2437,32 @@
         <v>50</v>
       </c>
       <c r="D58" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D59" t="s">
+        <v>189</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" t="s">
-        <v>179</v>
-      </c>
-      <c r="D59" t="s">
-        <v>190</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>23</v>
@@ -2453,32 +2471,32 @@
         <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>193</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" t="s">
         <v>194</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" t="s">
-        <v>90</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>6</v>
@@ -2487,32 +2505,32 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>199</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" t="s">
+        <v>201</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" t="s">
-        <v>90</v>
-      </c>
-      <c r="D63" t="s">
-        <v>202</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>6</v>
@@ -2521,32 +2539,32 @@
         <v>50</v>
       </c>
       <c r="D64" t="s">
+        <v>203</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>205</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D65" t="s">
         <v>206</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="E65" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>6</v>
@@ -2555,525 +2573,525 @@
         <v>50</v>
       </c>
       <c r="D66" t="s">
+        <v>209</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>211</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" t="s">
         <v>212</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67" t="s">
-        <v>90</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>214</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>178</v>
+      </c>
+      <c r="D68" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" t="s">
-        <v>179</v>
-      </c>
-      <c r="D68" t="s">
-        <v>218</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D69" t="s">
+        <v>218</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>89</v>
+      </c>
+      <c r="D70" t="s">
         <v>221</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" t="s">
-        <v>90</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E70" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>178</v>
+      </c>
+      <c r="D71" t="s">
         <v>224</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" t="s">
-        <v>179</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>229</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
         <v>230</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>231</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>233</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
         <v>234</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>235</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
         <v>241</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
+        <v>243</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="D76" t="s">
-        <v>244</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>244</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
         <v>245</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>246</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>248</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>245</v>
+      </c>
+      <c r="D78" t="s">
+        <v>250</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C78" t="s">
-        <v>246</v>
-      </c>
-      <c r="D78" t="s">
-        <v>251</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>251</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>178</v>
+      </c>
+      <c r="D79" t="s">
         <v>252</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" t="s">
-        <v>179</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="E79" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>254</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
+        <v>241</v>
+      </c>
+      <c r="D80" t="s">
         <v>255</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" t="s">
-        <v>242</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="E80" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>257</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>245</v>
+      </c>
+      <c r="D81" t="s">
         <v>258</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" t="s">
-        <v>246</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C82" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D82" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D83" t="s">
+        <v>264</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D84" t="s">
+        <v>267</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>269</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>234</v>
+      </c>
+      <c r="D85" t="s">
         <v>270</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" t="s">
-        <v>235</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>272</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>234</v>
+      </c>
+      <c r="D86" t="s">
         <v>273</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>235</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D87" t="s">
+        <v>276</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D88" t="s">
+        <v>279</v>
+      </c>
+      <c r="E88" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>281</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>178</v>
+      </c>
+      <c r="D89" t="s">
         <v>282</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>179</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>283</v>
-      </c>
-      <c r="E89" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" t="s">
+        <v>245</v>
+      </c>
+      <c r="D90" t="s">
         <v>285</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>246</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D91" t="s">
+        <v>288</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>290</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" t="s">
+        <v>245</v>
+      </c>
+      <c r="D92" t="s">
+        <v>292</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" t="s">
-        <v>246</v>
-      </c>
-      <c r="D92" t="s">
-        <v>293</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>293</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93" t="s">
+        <v>295</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C93" t="s">
-        <v>179</v>
-      </c>
-      <c r="D93" t="s">
-        <v>296</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>296</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>89</v>
+      </c>
+      <c r="D94" t="s">
         <v>297</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" t="s">
-        <v>90</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E94" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>299</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>245</v>
+      </c>
+      <c r="D95" t="s">
         <v>300</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" t="s">
-        <v>246</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E95" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>302</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>89</v>
+      </c>
+      <c r="D96" t="s">
         <v>303</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C96" t="s">
-        <v>90</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="E96" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>23</v>
@@ -3082,49 +3100,49 @@
         <v>24</v>
       </c>
       <c r="D97" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>308</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" t="s">
         <v>309</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" t="s">
-        <v>90</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C99" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D99" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>23</v>
@@ -3133,32 +3151,32 @@
         <v>24</v>
       </c>
       <c r="D100" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C101" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D101" t="s">
+        <v>318</v>
+      </c>
+      <c r="E101" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>6</v>
@@ -3167,32 +3185,32 @@
         <v>24</v>
       </c>
       <c r="D102" t="s">
+        <v>321</v>
+      </c>
+      <c r="E102" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>323</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" t="s">
         <v>324</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103" t="s">
-        <v>90</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="E103" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>6</v>
@@ -3201,44 +3219,78 @@
         <v>24</v>
       </c>
       <c r="D104" t="s">
+        <v>327</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C105" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C106" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D106" t="s">
+        <v>333</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E106" s="3" t="s">
-        <v>335</v>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>336</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" t="s">
+        <v>75</v>
+      </c>
+      <c r="D107" t="s">
+        <v>337</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>339</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>340</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3346,11 +3398,13 @@
     <hyperlink ref="E104" r:id="rId101" xr:uid="{0E450A26-1D93-4612-9D4A-FD1E5D2CEF6C}"/>
     <hyperlink ref="E105" r:id="rId102" xr:uid="{ED05E0E4-D757-405E-A527-46E3B16D41A6}"/>
     <hyperlink ref="E106" r:id="rId103" xr:uid="{1CF22A4F-D258-45B2-ABBD-F76220634F81}"/>
+    <hyperlink ref="E107" r:id="rId104" xr:uid="{317456F3-CC04-4C80-925A-F23EF607A64D}"/>
+    <hyperlink ref="E108" r:id="rId105" xr:uid="{B21FE459-5943-4A81-B3D0-FABB065886C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId104"/>
+  <pageSetup orientation="portrait" r:id="rId106"/>
   <tableParts count="1">
-    <tablePart r:id="rId105"/>
+    <tablePart r:id="rId107"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa begin top interview 150
</commit_message>
<xml_diff>
--- a/java/NC150.xlsx
+++ b/java/NC150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82E8164-83C1-45A7-85DB-7362A43E3605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E579F52-C5FE-4207-8655-0F5B65A9AF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B91" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>